<commit_message>
Correcion del archivo Excel de prueba
</commit_message>
<xml_diff>
--- a/ExcelDatosPrueba.xlsx
+++ b/ExcelDatosPrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4339E76C-3E66-4D7C-93B6-15BF1B013746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04B67AE-1CC1-4B86-AEDE-60501C5AE49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="2430" windowWidth="21600" windowHeight="11850" xr2:uid="{1F90918D-6BF3-419B-8ADD-5E40AF1E13ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1F90918D-6BF3-419B-8ADD-5E40AF1E13ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t xml:space="preserve">AÑO </t>
   </si>
@@ -87,10 +87,10 @@
     <t>2023.2</t>
   </si>
   <si>
-    <t>JuanEdufeedbackAI55555M</t>
-  </si>
-  <si>
-    <t>Profesor responsable</t>
+    <t>Juan - EdufeedbackAI - 55555M</t>
+  </si>
+  <si>
+    <t>CEDULA</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +534,9 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -566,6 +569,9 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -598,13 +604,16 @@
       <c r="J3">
         <v>1</v>
       </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -630,37 +639,8 @@
       <c r="J4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2023</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
+      <c r="K4">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>